<commit_message>
New changes to challange3
</commit_message>
<xml_diff>
--- a/SeleniumCodingChallangeSeries/src/main/java/SeleniumCodingChallange_TestData/SeleniumCodingChallangeSeries_3.xlsx
+++ b/SeleniumCodingChallangeSeries/src/main/java/SeleniumCodingChallange_TestData/SeleniumCodingChallangeSeries_3.xlsx
@@ -1,21 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Javaprogramming\codingchallange\coding-challange\SeleniumCodingChallangeSeries\src\main\java\SeleniumCodingChallange_TestData\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+  <workbookPr/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{E80B2E2E-E928-48B4-B525-D0109AC0D748}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11100" windowHeight="5985" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13060" windowHeight="5090" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LoginPage_3" sheetId="1" r:id="rId1"/>
     <sheet name="PeopleAndOrganisationsPage" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -132,7 +129,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -459,20 +456,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -480,7 +477,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -495,28 +492,28 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="Q1" sqref="Q1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.453125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.81640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.54296875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="20" bestFit="1" customWidth="1"/>
     <col min="11" max="12" width="11" customWidth="1"/>
     <col min="14" max="14" width="15" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>24</v>
       </c>
@@ -569,7 +566,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -624,7 +621,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="I2" r:id="rId1"/>
+    <hyperlink ref="I2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>

</xml_diff>

<commit_message>
data driven  changes added
</commit_message>
<xml_diff>
--- a/SeleniumCodingChallangeSeries/src/main/java/SeleniumCodingChallange_TestData/SeleniumCodingChallangeSeries_3.xlsx
+++ b/SeleniumCodingChallangeSeries/src/main/java/SeleniumCodingChallange_TestData/SeleniumCodingChallangeSeries_3.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{E80B2E2E-E928-48B4-B525-D0109AC0D748}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{2885EDBB-CF0B-4782-88DE-87AC2196835D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="13060" windowHeight="5090" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -495,9 +495,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>

</xml_diff>

<commit_message>
changes in test calass
</commit_message>
<xml_diff>
--- a/SeleniumCodingChallangeSeries/src/main/java/SeleniumCodingChallange_TestData/SeleniumCodingChallangeSeries_3.xlsx
+++ b/SeleniumCodingChallangeSeries/src/main/java/SeleniumCodingChallange_TestData/SeleniumCodingChallangeSeries_3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\parag.borawake\git\coding-challange\SeleniumCodingChallangeSeries\src\main\java\SeleniumCodingChallange_TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4B0562A-7BA7-44BC-A2C2-7B16D6944753}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80D7ECAA-B14E-43A9-BAE3-EE662436C58E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="13070" windowHeight="5090" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -500,7 +500,7 @@
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -513,6 +513,7 @@
     <col min="9" max="9" width="15.54296875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="20" bestFit="1" customWidth="1"/>
     <col min="11" max="12" width="11" customWidth="1"/>
+    <col min="13" max="13" width="9.36328125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="15" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="12" bestFit="1" customWidth="1"/>
   </cols>

</xml_diff>